<commit_message>
Completed CSV files for all product types
</commit_message>
<xml_diff>
--- a/Data/vendors.xlsx
+++ b/Data/vendors.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>High Khalid Limited</t>
   </si>
@@ -45,6 +45,60 @@
   </si>
   <si>
     <t>Abid Computers</t>
+  </si>
+  <si>
+    <t>Qazi and Kazi Brothers</t>
+  </si>
+  <si>
+    <t>Alam Gamerz</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Saddar</t>
+  </si>
+  <si>
+    <t>University Avenue</t>
+  </si>
+  <si>
+    <t>Sir Syed</t>
+  </si>
+  <si>
+    <t>Shop - 47, Technocity</t>
+  </si>
+  <si>
+    <t>Shop - 48, Technocity</t>
+  </si>
+  <si>
+    <t>Shop - 49, Technocity</t>
+  </si>
+  <si>
+    <t>Shop - 68, Technocity</t>
+  </si>
+  <si>
+    <t>Shop - 69, Technocity</t>
+  </si>
+  <si>
+    <t>Baithak, Habib University</t>
+  </si>
+  <si>
+    <t>Presidential Suite, Habib University</t>
+  </si>
+  <si>
+    <t>Shop C57, Sir Syed Road</t>
+  </si>
+  <si>
+    <t>Shop C52, Sir Syed Road</t>
   </si>
 </sst>
 </file>
@@ -362,47 +416,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F4:F12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F4:F12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F10" t="s">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F11" t="s">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F12" t="s">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>